<commit_message>
format data to table
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="train_horn" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -1201,6 +1201,26 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H73" totalsRowShown="0">
+  <autoFilter ref="A1:H73"/>
+  <sortState ref="A2:H73">
+    <sortCondition ref="A1:A73"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Reference"/>
+    <tableColumn id="2" name=" Value"/>
+    <tableColumn id="3" name=" Footprint"/>
+    <tableColumn id="4" name=" Datasheet"/>
+    <tableColumn id="5" name=" Manufacture"/>
+    <tableColumn id="6" name=" Mfg Part Number"/>
+    <tableColumn id="7" name=" Package"/>
+    <tableColumn id="8" name=" Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1489,12 +1509,12 @@
   <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="99.140625" bestFit="1" customWidth="1"/>
@@ -1532,142 +1552,166 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
+        <v>62</v>
+      </c>
+      <c r="B2">
+        <v>18650</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3">
+        <v>805</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>156</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>157</v>
       </c>
       <c r="G4">
         <v>805</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>157</v>
       </c>
       <c r="G5">
         <v>805</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>156</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="G6">
         <v>805</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>200</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7">
+        <v>805</v>
+      </c>
+      <c r="H7" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
         <v>43</v>
@@ -1679,174 +1723,174 @@
         <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="G8">
         <v>805</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>198</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>157</v>
       </c>
       <c r="G9">
         <v>805</v>
       </c>
       <c r="H9" t="s">
-        <v>51</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10">
-        <v>470</v>
+        <v>201</v>
+      </c>
+      <c r="B10" t="s">
+        <v>156</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>157</v>
       </c>
       <c r="G10">
         <v>805</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="G11">
         <v>805</v>
       </c>
       <c r="H11" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12">
-        <v>18650</v>
+        <v>119</v>
+      </c>
+      <c r="B12" t="s">
+        <v>116</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" t="s">
-        <v>19</v>
+        <v>117</v>
+      </c>
+      <c r="G12">
+        <v>805</v>
       </c>
       <c r="H12" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>208</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" t="s">
-        <v>74</v>
+        <v>117</v>
+      </c>
+      <c r="G13">
+        <v>805</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" t="s">
-        <v>80</v>
+        <v>157</v>
+      </c>
+      <c r="G14">
+        <v>805</v>
       </c>
       <c r="H14" t="s">
-        <v>81</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>209</v>
       </c>
       <c r="B15" t="s">
         <v>83</v>
@@ -1872,133 +1916,166 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" t="s">
-        <v>91</v>
+        <v>84</v>
+      </c>
+      <c r="G16">
+        <v>805</v>
       </c>
       <c r="H16" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>187</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="G17">
         <v>805</v>
       </c>
       <c r="H17" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>190</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
-      </c>
-      <c r="G18" t="s">
-        <v>19</v>
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18">
+        <v>805</v>
       </c>
       <c r="H18" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>191</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
-      </c>
-      <c r="G19" t="s">
-        <v>19</v>
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" t="s">
+        <v>157</v>
+      </c>
+      <c r="G19">
+        <v>805</v>
       </c>
       <c r="H19" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>189</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20">
+        <v>805</v>
+      </c>
+      <c r="H20" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>193</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>156</v>
       </c>
       <c r="C21" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F21" t="s">
-        <v>112</v>
-      </c>
-      <c r="G21" t="s">
-        <v>113</v>
+        <v>157</v>
+      </c>
+      <c r="G21">
+        <v>805</v>
       </c>
       <c r="H21" t="s">
-        <v>114</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>196</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="C22" t="s">
         <v>43</v>
@@ -2010,333 +2087,366 @@
         <v>45</v>
       </c>
       <c r="F22" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="G22">
         <v>805</v>
       </c>
       <c r="H22" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="F23" t="s">
-        <v>117</v>
+        <v>60</v>
       </c>
       <c r="G23">
         <v>805</v>
       </c>
       <c r="H23" t="s">
-        <v>118</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="F24" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="G24">
         <v>805</v>
       </c>
       <c r="H24" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="D25" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="E25" t="s">
-        <v>127</v>
+        <v>59</v>
       </c>
       <c r="F25" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="G25">
         <v>805</v>
       </c>
       <c r="H25" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>130</v>
+        <v>68</v>
       </c>
       <c r="B26" t="s">
-        <v>131</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
-        <v>133</v>
+        <v>72</v>
       </c>
       <c r="F26" t="s">
-        <v>134</v>
+        <v>73</v>
       </c>
       <c r="G26" t="s">
-        <v>135</v>
+        <v>74</v>
       </c>
       <c r="H26" t="s">
-        <v>136</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="B27" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" t="s">
-        <v>139</v>
-      </c>
-      <c r="E27" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" t="s">
-        <v>140</v>
-      </c>
-      <c r="G27">
-        <v>805</v>
+        <v>100</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
       </c>
       <c r="H27" t="s">
-        <v>141</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="B28" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="C28" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="D28" t="s">
-        <v>145</v>
+        <v>24</v>
       </c>
       <c r="E28" t="s">
-        <v>146</v>
+        <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>147</v>
-      </c>
-      <c r="G28" t="s">
-        <v>148</v>
+        <v>173</v>
+      </c>
+      <c r="G28">
+        <v>1206</v>
       </c>
       <c r="H28" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" t="s">
-        <v>152</v>
-      </c>
-      <c r="F29" t="s">
-        <v>153</v>
-      </c>
-      <c r="G29">
-        <v>805</v>
+        <v>104</v>
+      </c>
+      <c r="G29" t="s">
+        <v>19</v>
       </c>
       <c r="H29" t="s">
-        <v>154</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="B30" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" t="s">
-        <v>44</v>
+        <v>172</v>
       </c>
       <c r="E30" t="s">
-        <v>45</v>
+        <v>177</v>
       </c>
       <c r="F30" t="s">
-        <v>157</v>
-      </c>
-      <c r="G30">
-        <v>805</v>
+        <v>177</v>
+      </c>
+      <c r="G30" t="s">
+        <v>177</v>
       </c>
       <c r="H30" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>159</v>
+        <v>182</v>
       </c>
       <c r="B31" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="C31" t="s">
-        <v>161</v>
+        <v>172</v>
+      </c>
+      <c r="E31" t="s">
+        <v>177</v>
+      </c>
+      <c r="F31" t="s">
+        <v>177</v>
+      </c>
+      <c r="G31" t="s">
+        <v>177</v>
+      </c>
+      <c r="H31" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B32" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="C32" t="s">
-        <v>161</v>
+        <v>172</v>
+      </c>
+      <c r="E32" t="s">
+        <v>177</v>
+      </c>
+      <c r="F32" t="s">
+        <v>177</v>
+      </c>
+      <c r="G32" t="s">
+        <v>177</v>
+      </c>
+      <c r="H32" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="B33" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="C33" t="s">
-        <v>161</v>
+        <v>172</v>
+      </c>
+      <c r="E33" t="s">
+        <v>177</v>
+      </c>
+      <c r="F33" t="s">
+        <v>177</v>
+      </c>
+      <c r="G33" t="s">
+        <v>177</v>
+      </c>
+      <c r="H33" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c r="B34" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C34" t="s">
-        <v>161</v>
+        <v>172</v>
+      </c>
+      <c r="E34" t="s">
+        <v>177</v>
+      </c>
+      <c r="F34" t="s">
+        <v>177</v>
+      </c>
+      <c r="G34" t="s">
+        <v>177</v>
+      </c>
+      <c r="H34" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="B35" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C35" t="s">
-        <v>161</v>
+        <v>172</v>
+      </c>
+      <c r="E35" t="s">
+        <v>177</v>
+      </c>
+      <c r="F35" t="s">
+        <v>177</v>
+      </c>
+      <c r="G35" t="s">
+        <v>177</v>
+      </c>
+      <c r="H35" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>170</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>171</v>
+        <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>172</v>
-      </c>
-      <c r="D36" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" t="s">
-        <v>173</v>
-      </c>
-      <c r="G36">
-        <v>1206</v>
+        <v>18</v>
+      </c>
+      <c r="G36" t="s">
+        <v>19</v>
       </c>
       <c r="H36" t="s">
-        <v>174</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>175</v>
+        <v>142</v>
       </c>
       <c r="B37" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="C37" t="s">
-        <v>172</v>
+        <v>144</v>
+      </c>
+      <c r="D37" t="s">
+        <v>145</v>
       </c>
       <c r="E37" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="F37" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="G37" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="H37" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>178</v>
+        <v>120</v>
       </c>
       <c r="B38" t="s">
-        <v>179</v>
+        <v>121</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
@@ -2348,162 +2458,177 @@
         <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>180</v>
+        <v>122</v>
       </c>
       <c r="G38">
         <v>805</v>
       </c>
       <c r="H38" t="s">
-        <v>181</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>182</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>176</v>
+        <v>29</v>
       </c>
       <c r="C39" t="s">
-        <v>172</v>
+        <v>23</v>
+      </c>
+      <c r="D39" t="s">
+        <v>30</v>
       </c>
       <c r="E39" t="s">
-        <v>177</v>
+        <v>31</v>
       </c>
       <c r="F39" t="s">
-        <v>177</v>
-      </c>
-      <c r="G39" t="s">
-        <v>177</v>
+        <v>32</v>
+      </c>
+      <c r="G39">
+        <v>805</v>
       </c>
       <c r="H39" t="s">
-        <v>177</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="B40" t="s">
-        <v>176</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>172</v>
+        <v>23</v>
+      </c>
+      <c r="D40" t="s">
+        <v>24</v>
       </c>
       <c r="E40" t="s">
-        <v>177</v>
+        <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>177</v>
-      </c>
-      <c r="G40" t="s">
-        <v>177</v>
+        <v>36</v>
+      </c>
+      <c r="G40">
+        <v>805</v>
       </c>
       <c r="H40" t="s">
-        <v>177</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="B41" t="s">
-        <v>176</v>
+        <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>172</v>
+        <v>23</v>
+      </c>
+      <c r="D41" t="s">
+        <v>24</v>
       </c>
       <c r="E41" t="s">
-        <v>177</v>
+        <v>25</v>
       </c>
       <c r="F41" t="s">
-        <v>177</v>
-      </c>
-      <c r="G41" t="s">
-        <v>177</v>
+        <v>26</v>
+      </c>
+      <c r="G41">
+        <v>805</v>
       </c>
       <c r="H41" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="B42" t="s">
-        <v>176</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>172</v>
+        <v>23</v>
+      </c>
+      <c r="D42" t="s">
+        <v>30</v>
       </c>
       <c r="E42" t="s">
-        <v>177</v>
+        <v>31</v>
       </c>
       <c r="F42" t="s">
-        <v>177</v>
-      </c>
-      <c r="G42" t="s">
-        <v>177</v>
+        <v>32</v>
+      </c>
+      <c r="G42">
+        <v>805</v>
       </c>
       <c r="H42" t="s">
-        <v>177</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="B43" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="C43" t="s">
-        <v>172</v>
+        <v>23</v>
+      </c>
+      <c r="D43" t="s">
+        <v>24</v>
       </c>
       <c r="E43" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="F43" t="s">
-        <v>177</v>
-      </c>
-      <c r="G43" t="s">
-        <v>177</v>
+        <v>153</v>
+      </c>
+      <c r="G43">
+        <v>805</v>
       </c>
       <c r="H43" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D44" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E44" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="G44">
         <v>805</v>
       </c>
       <c r="H44" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="B45" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="C45" t="s">
         <v>23</v>
@@ -2515,359 +2640,359 @@
         <v>25</v>
       </c>
       <c r="F45" t="s">
-        <v>122</v>
+        <v>26</v>
       </c>
       <c r="G45">
         <v>805</v>
       </c>
       <c r="H45" t="s">
-        <v>123</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D46" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E46" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F46" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="G46">
         <v>805</v>
       </c>
       <c r="H46" t="s">
-        <v>85</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>179</v>
       </c>
       <c r="C47" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E47" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F47" t="s">
-        <v>84</v>
+        <v>180</v>
       </c>
       <c r="G47">
         <v>805</v>
       </c>
       <c r="H47" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="B48" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="C48" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D48" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E48" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F48" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="G48">
         <v>805</v>
       </c>
       <c r="H48" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>192</v>
+        <v>124</v>
       </c>
       <c r="B49" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="C49" t="s">
         <v>23</v>
       </c>
       <c r="D49" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="E49" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="F49" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="G49">
         <v>805</v>
       </c>
       <c r="H49" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="B50" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="C50" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D50" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E50" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F50" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="G50">
         <v>805</v>
       </c>
       <c r="H50" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="B51" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="C51" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D51" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E51" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F51" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="G51">
         <v>805</v>
       </c>
       <c r="H51" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="B52" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="C52" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D52" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E52" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F52" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="G52">
         <v>805</v>
       </c>
       <c r="H52" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>196</v>
+        <v>214</v>
       </c>
       <c r="B53" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="C53" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D53" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E53" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F53" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="G53">
         <v>805</v>
       </c>
       <c r="H53" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="B54" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="C54" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D54" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E54" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F54" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="G54">
         <v>805</v>
       </c>
       <c r="H54" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="B55" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="C55" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D55" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E55" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F55" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="G55">
         <v>805</v>
       </c>
       <c r="H55" t="s">
-        <v>158</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>199</v>
-      </c>
-      <c r="B56" t="s">
-        <v>156</v>
+        <v>52</v>
+      </c>
+      <c r="B56">
+        <v>470</v>
       </c>
       <c r="C56" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D56" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E56" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F56" t="s">
-        <v>157</v>
+        <v>53</v>
       </c>
       <c r="G56">
         <v>805</v>
       </c>
       <c r="H56" t="s">
-        <v>158</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="B57" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="C57" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D57" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E57" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F57" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="G57">
         <v>805</v>
       </c>
       <c r="H57" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>201</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D58" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E58" t="s">
-        <v>45</v>
+        <v>152</v>
       </c>
       <c r="F58" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G58">
         <v>805</v>
       </c>
       <c r="H58" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>202</v>
+        <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C59" t="s">
         <v>23</v>
@@ -2879,47 +3004,32 @@
         <v>25</v>
       </c>
       <c r="F59" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="G59">
         <v>805</v>
       </c>
       <c r="H59" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>203</v>
+        <v>106</v>
       </c>
       <c r="B60" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="C60" t="s">
         <v>23</v>
       </c>
-      <c r="D60" t="s">
-        <v>24</v>
-      </c>
-      <c r="E60" t="s">
-        <v>25</v>
-      </c>
-      <c r="F60" t="s">
-        <v>36</v>
-      </c>
-      <c r="G60">
-        <v>805</v>
-      </c>
-      <c r="H60" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>204</v>
+        <v>34</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C61" t="s">
         <v>23</v>
@@ -2931,18 +3041,18 @@
         <v>25</v>
       </c>
       <c r="F61" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="G61">
         <v>805</v>
       </c>
       <c r="H61" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>205</v>
+        <v>21</v>
       </c>
       <c r="B62" t="s">
         <v>22</v>
@@ -2968,291 +3078,205 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>206</v>
+        <v>86</v>
       </c>
       <c r="B63" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="C63" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="D63" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="E63" t="s">
         <v>31</v>
       </c>
       <c r="F63" t="s">
-        <v>32</v>
-      </c>
-      <c r="G63">
-        <v>805</v>
+        <v>90</v>
+      </c>
+      <c r="G63" t="s">
+        <v>91</v>
       </c>
       <c r="H63" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>207</v>
+        <v>159</v>
       </c>
       <c r="B64" t="s">
-        <v>29</v>
+        <v>160</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
-      </c>
-      <c r="D64" t="s">
-        <v>30</v>
-      </c>
-      <c r="E64" t="s">
-        <v>31</v>
-      </c>
-      <c r="F64" t="s">
-        <v>32</v>
-      </c>
-      <c r="G64">
-        <v>805</v>
-      </c>
-      <c r="H64" t="s">
-        <v>33</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>208</v>
+        <v>162</v>
       </c>
       <c r="B65" t="s">
-        <v>116</v>
+        <v>163</v>
       </c>
       <c r="C65" t="s">
-        <v>43</v>
-      </c>
-      <c r="D65" t="s">
-        <v>44</v>
-      </c>
-      <c r="E65" t="s">
-        <v>45</v>
-      </c>
-      <c r="F65" t="s">
-        <v>117</v>
-      </c>
-      <c r="G65">
-        <v>805</v>
-      </c>
-      <c r="H65" t="s">
-        <v>118</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>209</v>
+        <v>164</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
       <c r="C66" t="s">
-        <v>43</v>
-      </c>
-      <c r="D66" t="s">
-        <v>44</v>
-      </c>
-      <c r="E66" t="s">
-        <v>45</v>
-      </c>
-      <c r="F66" t="s">
-        <v>84</v>
-      </c>
-      <c r="G66">
-        <v>805</v>
-      </c>
-      <c r="H66" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>210</v>
+        <v>166</v>
       </c>
       <c r="B67" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C67" t="s">
-        <v>23</v>
-      </c>
-      <c r="D67" t="s">
-        <v>24</v>
-      </c>
-      <c r="E67" t="s">
-        <v>25</v>
-      </c>
-      <c r="F67" t="s">
-        <v>180</v>
-      </c>
-      <c r="G67">
-        <v>805</v>
-      </c>
-      <c r="H67" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>211</v>
+        <v>168</v>
       </c>
       <c r="B68" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C68" t="s">
-        <v>23</v>
-      </c>
-      <c r="D68" t="s">
-        <v>24</v>
-      </c>
-      <c r="E68" t="s">
-        <v>25</v>
-      </c>
-      <c r="F68" t="s">
-        <v>180</v>
-      </c>
-      <c r="G68">
-        <v>805</v>
-      </c>
-      <c r="H68" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>212</v>
+        <v>130</v>
       </c>
       <c r="B69" t="s">
-        <v>179</v>
+        <v>131</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D69" t="s">
-        <v>24</v>
+        <v>132</v>
       </c>
       <c r="E69" t="s">
-        <v>25</v>
+        <v>133</v>
       </c>
       <c r="F69" t="s">
-        <v>180</v>
-      </c>
-      <c r="G69">
-        <v>805</v>
+        <v>134</v>
+      </c>
+      <c r="G69" t="s">
+        <v>135</v>
       </c>
       <c r="H69" t="s">
-        <v>181</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>213</v>
+        <v>38</v>
       </c>
       <c r="B70" t="s">
-        <v>179</v>
+        <v>39</v>
       </c>
       <c r="C70" t="s">
-        <v>23</v>
-      </c>
-      <c r="D70" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" t="s">
-        <v>25</v>
-      </c>
-      <c r="F70" t="s">
-        <v>180</v>
-      </c>
-      <c r="G70">
-        <v>805</v>
-      </c>
-      <c r="H70" t="s">
-        <v>181</v>
+        <v>40</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>214</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
-        <v>179</v>
+        <v>77</v>
       </c>
       <c r="C71" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="D71" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="E71" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F71" t="s">
-        <v>180</v>
-      </c>
-      <c r="G71">
-        <v>805</v>
+        <v>77</v>
+      </c>
+      <c r="G71" t="s">
+        <v>80</v>
       </c>
       <c r="H71" t="s">
-        <v>181</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>215</v>
+        <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>179</v>
+        <v>9</v>
       </c>
       <c r="C72" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D72" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E72" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F72" t="s">
-        <v>180</v>
-      </c>
-      <c r="G72">
-        <v>805</v>
+        <v>13</v>
+      </c>
+      <c r="G72" t="s">
+        <v>14</v>
       </c>
       <c r="H72" t="s">
-        <v>181</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>216</v>
+        <v>108</v>
       </c>
       <c r="B73" t="s">
-        <v>179</v>
+        <v>109</v>
       </c>
       <c r="C73" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="D73" t="s">
-        <v>24</v>
+        <v>111</v>
       </c>
       <c r="E73" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F73" t="s">
-        <v>180</v>
-      </c>
-      <c r="G73">
-        <v>805</v>
+        <v>112</v>
+      </c>
+      <c r="G73" t="s">
+        <v>113</v>
       </c>
       <c r="H73" t="s">
-        <v>181</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update BOM with corrected fields
Removed TP from bom list
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="train_horn" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="206">
   <si>
     <t>Reference</t>
   </si>
@@ -106,186 +106,183 @@
     <t>3.6k</t>
   </si>
   <si>
-    <t>https://industrial.panasonic.com/cdbs/www-data/pdf/RDM0000/AOA0000C307.pdf</t>
+    <t>RC0805FR-073K6L</t>
+  </si>
+  <si>
+    <t>RES SMD 3.6K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>6.2k</t>
+  </si>
+  <si>
+    <t>RC0805FR-076K2L</t>
+  </si>
+  <si>
+    <t>RES SMD 6.2K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>MCP73831</t>
+  </si>
+  <si>
+    <t>TO_SOT_Packages_SMD:SOT-23-5</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>4.7uF</t>
+  </si>
+  <si>
+    <t>Capacitors_SMD:C_0805</t>
+  </si>
+  <si>
+    <t>https://media.digikey.com/pdf/Data%20Sheets/Samsung%20PDFs/CL_Series_MLCC_ds.pdf</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>CL21A475KQFNNNG</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 6.3V X5R 0805</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>RC0805FR-072KL</t>
+  </si>
+  <si>
+    <t>RES SMD 2K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>RC0805FR-07470RL</t>
+  </si>
+  <si>
+    <t>RES SMD 470 OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>lib_fp:LED_0805_LIGHTPIPE</t>
+  </si>
+  <si>
+    <t>http://katalog.we-online.de/led/datasheet/150080BS75000.pdf</t>
+  </si>
+  <si>
+    <t>Wurth Electronics Inc.</t>
+  </si>
+  <si>
+    <t>150080BS75000</t>
+  </si>
+  <si>
+    <t>Blue 470nm LED Indication</t>
+  </si>
+  <si>
+    <t>BT1</t>
+  </si>
+  <si>
+    <t>lib_fp:18650_battery_holder_PCB_Pins</t>
+  </si>
+  <si>
+    <t>http://www.memoryprotectiondevices.com/datasheets/BH-18650-PC-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>MPD</t>
+  </si>
+  <si>
+    <t>BH-18650-PC-ND</t>
+  </si>
+  <si>
+    <t>HOLDER BATT 18650 1CELL PC PIN</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>USB_OTG</t>
+  </si>
+  <si>
+    <t>lib_fp:USB_Micro-B_Amphenol_10118192-0001LF</t>
+  </si>
+  <si>
+    <t>https://cdn.amphenol-icc.com/media/wysiwyg/files/drawing/10118192.pdf</t>
+  </si>
+  <si>
+    <t>Amphenol</t>
+  </si>
+  <si>
+    <t>10118192-0001LF</t>
+  </si>
+  <si>
+    <t>USB MICRO B</t>
+  </si>
+  <si>
+    <t>CONN USB MICRO B RECPT SMT R/A</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>TPS78233DDCR</t>
+  </si>
+  <si>
+    <t>TO_SOT_Packages_SMD:TSOT-23-5</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/tps782.pdf</t>
+  </si>
+  <si>
+    <t>SOT23-5</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V 150MA SOT23-5</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>CL21B105KOFNNNG</t>
+  </si>
+  <si>
+    <t>CAP CER 1UF 16V X7R 0805</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>PLAY</t>
+  </si>
+  <si>
+    <t>lib_fp:SWITCH_Panasonic_SMDRight_EVQP7C</t>
+  </si>
+  <si>
+    <t>https://www3.panasonic.biz/ac/e_download/control/switch/light-touch/catalog/sw_lt_eng_3529s_side.pdf</t>
   </si>
   <si>
     <t>Panasonic Electronic Components</t>
   </si>
   <si>
-    <t>ERA-6AEB362V</t>
-  </si>
-  <si>
-    <t>RES SMD 3.6K OHM 0.1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
-    <t>6.2k</t>
-  </si>
-  <si>
-    <t>RC0805FR-076K2L</t>
-  </si>
-  <si>
-    <t>RES SMD 6.2K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>MCP73831</t>
-  </si>
-  <si>
-    <t>TO_SOT_Packages_SMD:SOT-23-5</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
-    <t>Capacitors_SMD:C_0805</t>
-  </si>
-  <si>
-    <t>https://media.digikey.com/pdf/Data%20Sheets/Samsung%20PDFs/CL_Series_MLCC_ds.pdf</t>
-  </si>
-  <si>
-    <t>Samsung Electro-Mechanics</t>
-  </si>
-  <si>
-    <t>CL21A475KQFNNNG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.7ÂµF Â±10% 6.3V Ceramic Capacitor X5R 0805 </t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>2k</t>
-  </si>
-  <si>
-    <t>RC0805FR-072KL</t>
-  </si>
-  <si>
-    <t>RES SMD 2K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>RC0805FR-07470RL</t>
-  </si>
-  <si>
-    <t>RES SMD 470 OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>BLUE</t>
-  </si>
-  <si>
-    <t>lib_fp:LED_0805_LIGHTPIPE</t>
-  </si>
-  <si>
-    <t>http://katalog.we-online.de/led/datasheet/150080BS75000.pdf</t>
-  </si>
-  <si>
-    <t>Wurth Electronics Inc.</t>
-  </si>
-  <si>
-    <t>150080BS75000</t>
-  </si>
-  <si>
-    <t>Blue 470nm LED Indication</t>
-  </si>
-  <si>
-    <t>BT1</t>
-  </si>
-  <si>
-    <t>lib_fp:18650_battery_holder_PCB_Pins</t>
-  </si>
-  <si>
-    <t>http://www.memoryprotectiondevices.com/datasheets/BH-18650-PC-datasheet.pdf</t>
-  </si>
-  <si>
-    <t>MPD</t>
-  </si>
-  <si>
-    <t>BH-18650-PC-ND</t>
-  </si>
-  <si>
-    <t>HOLDER BATT 18650 1CELL PC PIN</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>USB_OTG</t>
-  </si>
-  <si>
-    <t>lib_fp:USB_Micro-B_Amphenol_10118192-0001LF</t>
-  </si>
-  <si>
-    <t>https://cdn.amphenol-icc.com/media/wysiwyg/files/drawing/10118192.pdf</t>
-  </si>
-  <si>
-    <t>Amphenol</t>
-  </si>
-  <si>
-    <t>10118192-0001LF</t>
-  </si>
-  <si>
-    <t>USB MICRO B</t>
-  </si>
-  <si>
-    <t>USB - micro B USB 2.0 Receptacle Connector 5 Position Surface Mount, Right Angle</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>TPS78233DDCR</t>
-  </si>
-  <si>
-    <t>TO_SOT_Packages_SMD:TSOT-23-5</t>
-  </si>
-  <si>
-    <t>http://www.ti.com/lit/ds/symlink/tps782.pdf</t>
-  </si>
-  <si>
-    <t>SOT23-5</t>
-  </si>
-  <si>
-    <t>IC REG LINEAR 3.3V 150MA SOT23-5</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>CL21B105KOFNNNG</t>
-  </si>
-  <si>
-    <t>CAP CER 1UF 16V X7R 0805</t>
-  </si>
-  <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>PLAY</t>
-  </si>
-  <si>
-    <t>lib_fp:SWITCH_Panasonic_SMDRight_EVQP7C</t>
-  </si>
-  <si>
-    <t>https://www3.panasonic.biz/ac/e_download/control/switch/light-touch/catalog/sw_lt_eng_3529s_side.pdf</t>
-  </si>
-  <si>
     <t>EVQ-P7C01P</t>
   </si>
   <si>
@@ -340,6 +337,12 @@
     <t>47k</t>
   </si>
   <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>DO NOT POPULATE</t>
+  </si>
+  <si>
     <t>U5</t>
   </si>
   <si>
@@ -493,39 +496,6 @@
     <t>CAP CER 0.1UF 16V X7R 0805</t>
   </si>
   <si>
-    <t>TP1</t>
-  </si>
-  <si>
-    <t>P1.1</t>
-  </si>
-  <si>
-    <t>Connectors_TestPoints:Test_Point_Pad_d1.5mm</t>
-  </si>
-  <si>
-    <t>TP2</t>
-  </si>
-  <si>
-    <t>P1.4</t>
-  </si>
-  <si>
-    <t>TP3</t>
-  </si>
-  <si>
-    <t>P1.6</t>
-  </si>
-  <si>
-    <t>TP4</t>
-  </si>
-  <si>
-    <t>P2.6</t>
-  </si>
-  <si>
-    <t>TP5</t>
-  </si>
-  <si>
-    <t>P2.7</t>
-  </si>
-  <si>
     <t>JP1</t>
   </si>
   <si>
@@ -545,9 +515,6 @@
   </si>
   <si>
     <t>GADJ</t>
-  </si>
-  <si>
-    <t>NONE</t>
   </si>
   <si>
     <t>R18</t>
@@ -1202,8 +1169,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H73" totalsRowShown="0">
-  <autoFilter ref="A1:H73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H68" totalsRowShown="0">
+  <autoFilter ref="A1:H68"/>
   <sortState ref="A2:H73">
     <sortCondition ref="A1:A73"/>
   </sortState>
@@ -1506,22 +1473,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="99.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="74.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1552,680 +1519,680 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2">
         <v>18650</v>
       </c>
       <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>64</v>
-      </c>
-      <c r="E2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" t="s">
-        <v>66</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>44</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3">
+        <v>805</v>
+      </c>
+      <c r="H3" t="s">
         <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3">
-        <v>805</v>
-      </c>
-      <c r="H3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" t="s">
-        <v>45</v>
-      </c>
       <c r="F4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G4">
         <v>805</v>
       </c>
       <c r="H4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
         <v>43</v>
       </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
       <c r="F5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G5">
         <v>805</v>
       </c>
       <c r="H5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
         <v>43</v>
       </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
       <c r="F6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G6">
         <v>805</v>
       </c>
       <c r="H6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
       <c r="F7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G7">
         <v>805</v>
       </c>
       <c r="H7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" t="s">
-        <v>45</v>
-      </c>
       <c r="F8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G8">
         <v>805</v>
       </c>
       <c r="H8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
         <v>43</v>
       </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
       <c r="F9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G9">
         <v>805</v>
       </c>
       <c r="H9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
       <c r="F10" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G10">
         <v>805</v>
       </c>
       <c r="H10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
       <c r="F11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G11">
         <v>805</v>
       </c>
       <c r="H11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12">
+        <v>805</v>
+      </c>
+      <c r="H12" t="s">
         <v>119</v>
-      </c>
-      <c r="B12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" t="s">
-        <v>117</v>
-      </c>
-      <c r="G12">
-        <v>805</v>
-      </c>
-      <c r="H12" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
         <v>43</v>
       </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" t="s">
-        <v>45</v>
-      </c>
       <c r="F13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G13">
         <v>805</v>
       </c>
       <c r="H13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
         <v>43</v>
       </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" t="s">
-        <v>45</v>
-      </c>
       <c r="F14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G14">
         <v>805</v>
       </c>
       <c r="H14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15">
+        <v>805</v>
+      </c>
+      <c r="H15" t="s">
         <v>83</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15">
-        <v>805</v>
-      </c>
-      <c r="H15" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" t="s">
         <v>82</v>
       </c>
-      <c r="B16" t="s">
+      <c r="G16">
+        <v>805</v>
+      </c>
+      <c r="H16" t="s">
         <v>83</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16">
-        <v>805</v>
-      </c>
-      <c r="H16" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
         <v>42</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>43</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>44</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17">
+        <v>805</v>
+      </c>
+      <c r="H17" t="s">
         <v>45</v>
-      </c>
-      <c r="F17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17">
-        <v>805</v>
-      </c>
-      <c r="H17" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18">
+        <v>805</v>
+      </c>
+      <c r="H18" t="s">
         <v>83</v>
-      </c>
-      <c r="C18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18">
-        <v>805</v>
-      </c>
-      <c r="H18" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" t="s">
         <v>43</v>
       </c>
-      <c r="D19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" t="s">
-        <v>45</v>
-      </c>
       <c r="F19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G19">
         <v>805</v>
       </c>
       <c r="H19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20">
+        <v>805</v>
+      </c>
+      <c r="H20" t="s">
         <v>83</v>
-      </c>
-      <c r="C20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" t="s">
-        <v>84</v>
-      </c>
-      <c r="G20">
-        <v>805</v>
-      </c>
-      <c r="H20" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="B21" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" t="s">
         <v>43</v>
       </c>
-      <c r="D21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" t="s">
-        <v>45</v>
-      </c>
       <c r="F21" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G21">
         <v>805</v>
       </c>
       <c r="H21" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="B22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" t="s">
         <v>43</v>
       </c>
-      <c r="D22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" t="s">
-        <v>45</v>
-      </c>
       <c r="F22" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G22">
         <v>805</v>
       </c>
       <c r="H22" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
         <v>55</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>56</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
         <v>57</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F23" t="s">
         <v>58</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23">
+        <v>805</v>
+      </c>
+      <c r="H23" t="s">
         <v>59</v>
-      </c>
-      <c r="F23" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23">
-        <v>805</v>
-      </c>
-      <c r="H23" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>140</v>
+      </c>
+      <c r="E24" t="s">
         <v>57</v>
       </c>
-      <c r="D24" t="s">
-        <v>139</v>
-      </c>
-      <c r="E24" t="s">
-        <v>59</v>
-      </c>
       <c r="F24" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G24">
         <v>805</v>
       </c>
       <c r="H24" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
         <v>93</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
         <v>94</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>57</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
         <v>95</v>
       </c>
-      <c r="E25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="G25">
+        <v>805</v>
+      </c>
+      <c r="H25" t="s">
         <v>96</v>
-      </c>
-      <c r="G25">
-        <v>805</v>
-      </c>
-      <c r="H25" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
         <v>68</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>69</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>70</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>71</v>
       </c>
-      <c r="E26" t="s">
+      <c r="G26" t="s">
         <v>72</v>
       </c>
-      <c r="F26" t="s">
+      <c r="H26" t="s">
         <v>73</v>
-      </c>
-      <c r="G26" t="s">
-        <v>74</v>
-      </c>
-      <c r="H26" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
         <v>98</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>99</v>
-      </c>
-      <c r="C27" t="s">
-        <v>100</v>
       </c>
       <c r="G27" t="s">
         <v>19</v>
       </c>
       <c r="H27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B28" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="C28" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D28" t="s">
         <v>24</v>
@@ -2234,168 +2201,186 @@
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G28">
         <v>1206</v>
       </c>
       <c r="H28" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" t="s">
         <v>102</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>103</v>
-      </c>
-      <c r="C29" t="s">
-        <v>104</v>
       </c>
       <c r="G29" t="s">
         <v>19</v>
       </c>
       <c r="H29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B30" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C30" t="s">
-        <v>172</v>
+        <v>162</v>
+      </c>
+      <c r="D30" t="s">
+        <v>24</v>
       </c>
       <c r="E30" t="s">
-        <v>177</v>
+        <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>177</v>
-      </c>
-      <c r="G30" t="s">
-        <v>177</v>
+        <v>163</v>
+      </c>
+      <c r="G30">
+        <v>1206</v>
       </c>
       <c r="H30" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B31" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C31" t="s">
-        <v>172</v>
+        <v>162</v>
+      </c>
+      <c r="D31" t="s">
+        <v>24</v>
       </c>
       <c r="E31" t="s">
-        <v>177</v>
+        <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>177</v>
-      </c>
-      <c r="G31" t="s">
-        <v>177</v>
+        <v>163</v>
+      </c>
+      <c r="G31">
+        <v>1206</v>
       </c>
       <c r="H31" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B32" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C32" t="s">
-        <v>172</v>
+        <v>162</v>
+      </c>
+      <c r="D32" t="s">
+        <v>24</v>
       </c>
       <c r="E32" t="s">
-        <v>177</v>
+        <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>177</v>
-      </c>
-      <c r="G32" t="s">
-        <v>177</v>
+        <v>163</v>
+      </c>
+      <c r="G32">
+        <v>1206</v>
       </c>
       <c r="H32" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B33" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C33" t="s">
-        <v>172</v>
+        <v>162</v>
+      </c>
+      <c r="D33" t="s">
+        <v>24</v>
       </c>
       <c r="E33" t="s">
-        <v>177</v>
+        <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>177</v>
-      </c>
-      <c r="G33" t="s">
-        <v>177</v>
+        <v>163</v>
+      </c>
+      <c r="G33">
+        <v>1206</v>
       </c>
       <c r="H33" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B34" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C34" t="s">
-        <v>172</v>
+        <v>162</v>
+      </c>
+      <c r="D34" t="s">
+        <v>24</v>
       </c>
       <c r="E34" t="s">
-        <v>177</v>
+        <v>25</v>
       </c>
       <c r="F34" t="s">
-        <v>177</v>
-      </c>
-      <c r="G34" t="s">
-        <v>177</v>
+        <v>163</v>
+      </c>
+      <c r="G34">
+        <v>1206</v>
       </c>
       <c r="H34" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B35" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C35" t="s">
-        <v>172</v>
+        <v>162</v>
+      </c>
+      <c r="D35" t="s">
+        <v>24</v>
       </c>
       <c r="E35" t="s">
-        <v>177</v>
+        <v>25</v>
       </c>
       <c r="F35" t="s">
-        <v>177</v>
-      </c>
-      <c r="G35" t="s">
-        <v>177</v>
+        <v>163</v>
+      </c>
+      <c r="G35">
+        <v>1206</v>
       </c>
       <c r="H35" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2417,36 +2402,36 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B37" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C37" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D37" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E37" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F37" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G37" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H37" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B38" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C38" t="s">
         <v>23</v>
@@ -2458,13 +2443,13 @@
         <v>25</v>
       </c>
       <c r="F38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G38">
         <v>805</v>
       </c>
       <c r="H38" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2478,27 +2463,27 @@
         <v>23</v>
       </c>
       <c r="D39" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" t="s">
         <v>30</v>
       </c>
-      <c r="E39" t="s">
+      <c r="G39">
+        <v>805</v>
+      </c>
+      <c r="H39" t="s">
         <v>31</v>
-      </c>
-      <c r="F39" t="s">
-        <v>32</v>
-      </c>
-      <c r="G39">
-        <v>805</v>
-      </c>
-      <c r="H39" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C40" t="s">
         <v>23</v>
@@ -2510,18 +2495,18 @@
         <v>25</v>
       </c>
       <c r="F40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G40">
         <v>805</v>
       </c>
       <c r="H40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="B41" t="s">
         <v>22</v>
@@ -2547,7 +2532,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B42" t="s">
         <v>29</v>
@@ -2556,27 +2541,27 @@
         <v>23</v>
       </c>
       <c r="D42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" t="s">
         <v>30</v>
       </c>
-      <c r="E42" t="s">
+      <c r="G42">
+        <v>805</v>
+      </c>
+      <c r="H42" t="s">
         <v>31</v>
-      </c>
-      <c r="F42" t="s">
-        <v>32</v>
-      </c>
-      <c r="G42">
-        <v>805</v>
-      </c>
-      <c r="H42" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B43" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
@@ -2585,24 +2570,24 @@
         <v>24</v>
       </c>
       <c r="E43" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F43" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G43">
         <v>805</v>
       </c>
       <c r="H43" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C44" t="s">
         <v>23</v>
@@ -2614,18 +2599,18 @@
         <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G44">
         <v>805</v>
       </c>
       <c r="H44" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="B45" t="s">
         <v>22</v>
@@ -2651,7 +2636,7 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="B46" t="s">
         <v>29</v>
@@ -2660,27 +2645,27 @@
         <v>23</v>
       </c>
       <c r="D46" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" t="s">
         <v>30</v>
       </c>
-      <c r="E46" t="s">
+      <c r="G46">
+        <v>805</v>
+      </c>
+      <c r="H46" t="s">
         <v>31</v>
-      </c>
-      <c r="F46" t="s">
-        <v>32</v>
-      </c>
-      <c r="G46">
-        <v>805</v>
-      </c>
-      <c r="H46" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="B47" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C47" t="s">
         <v>23</v>
@@ -2692,21 +2677,21 @@
         <v>25</v>
       </c>
       <c r="F47" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="G47">
         <v>805</v>
       </c>
       <c r="H47" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B48" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C48" t="s">
         <v>23</v>
@@ -2718,47 +2703,47 @@
         <v>25</v>
       </c>
       <c r="F48" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="G48">
         <v>805</v>
       </c>
       <c r="H48" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B49" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C49" t="s">
         <v>23</v>
       </c>
       <c r="D49" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E49" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F49" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G49">
         <v>805</v>
       </c>
       <c r="H49" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B50" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C50" t="s">
         <v>23</v>
@@ -2770,21 +2755,21 @@
         <v>25</v>
       </c>
       <c r="F50" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="G50">
         <v>805</v>
       </c>
       <c r="H50" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="B51" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C51" t="s">
         <v>23</v>
@@ -2796,21 +2781,21 @@
         <v>25</v>
       </c>
       <c r="F51" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="G51">
         <v>805</v>
       </c>
       <c r="H51" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B52" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C52" t="s">
         <v>23</v>
@@ -2822,21 +2807,21 @@
         <v>25</v>
       </c>
       <c r="F52" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="G52">
         <v>805</v>
       </c>
       <c r="H52" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B53" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C53" t="s">
         <v>23</v>
@@ -2848,21 +2833,21 @@
         <v>25</v>
       </c>
       <c r="F53" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="G53">
         <v>805</v>
       </c>
       <c r="H53" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="B54" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C54" t="s">
         <v>23</v>
@@ -2874,21 +2859,21 @@
         <v>25</v>
       </c>
       <c r="F54" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="G54">
         <v>805</v>
       </c>
       <c r="H54" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="B55" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C55" t="s">
         <v>23</v>
@@ -2900,18 +2885,18 @@
         <v>25</v>
       </c>
       <c r="F55" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="G55">
         <v>805</v>
       </c>
       <c r="H55" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B56">
         <v>470</v>
@@ -2926,21 +2911,21 @@
         <v>25</v>
       </c>
       <c r="F56" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G56">
         <v>805</v>
       </c>
       <c r="H56" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B57" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C57" t="s">
         <v>23</v>
@@ -2952,21 +2937,21 @@
         <v>25</v>
       </c>
       <c r="F57" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G57">
         <v>805</v>
       </c>
       <c r="H57" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B58" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C58" t="s">
         <v>23</v>
@@ -2975,24 +2960,24 @@
         <v>24</v>
       </c>
       <c r="E58" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F58" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G58">
         <v>805</v>
       </c>
       <c r="H58" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B59" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C59" t="s">
         <v>23</v>
@@ -3004,32 +2989,44 @@
         <v>25</v>
       </c>
       <c r="F59" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G59">
         <v>805</v>
       </c>
       <c r="H59" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
+        <v>105</v>
+      </c>
+      <c r="B60" t="s">
         <v>106</v>
-      </c>
-      <c r="B60" t="s">
-        <v>107</v>
       </c>
       <c r="C60" t="s">
         <v>23</v>
       </c>
+      <c r="E60" t="s">
+        <v>107</v>
+      </c>
+      <c r="F60" t="s">
+        <v>107</v>
+      </c>
+      <c r="G60" t="s">
+        <v>107</v>
+      </c>
+      <c r="H60" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C61" t="s">
         <v>23</v>
@@ -3041,13 +3038,13 @@
         <v>25</v>
       </c>
       <c r="F61" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G61">
         <v>805</v>
       </c>
       <c r="H61" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -3078,198 +3075,143 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" t="s">
         <v>86</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D63" t="s">
         <v>87</v>
       </c>
-      <c r="C63" t="s">
+      <c r="E63" t="s">
         <v>88</v>
       </c>
-      <c r="D63" t="s">
+      <c r="F63" t="s">
         <v>89</v>
       </c>
-      <c r="E63" t="s">
-        <v>31</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>90</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>91</v>
-      </c>
-      <c r="H63" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="B64" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="C64" t="s">
-        <v>161</v>
+        <v>38</v>
+      </c>
+      <c r="D64" t="s">
+        <v>133</v>
+      </c>
+      <c r="E64" t="s">
+        <v>134</v>
+      </c>
+      <c r="F64" t="s">
+        <v>135</v>
+      </c>
+      <c r="G64" t="s">
+        <v>136</v>
+      </c>
+      <c r="H64" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>162</v>
+        <v>36</v>
       </c>
       <c r="B65" t="s">
-        <v>163</v>
+        <v>37</v>
       </c>
       <c r="C65" t="s">
-        <v>161</v>
+        <v>38</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>164</v>
+        <v>74</v>
       </c>
       <c r="B66" t="s">
-        <v>165</v>
+        <v>75</v>
       </c>
       <c r="C66" t="s">
-        <v>161</v>
+        <v>76</v>
+      </c>
+      <c r="D66" t="s">
+        <v>77</v>
+      </c>
+      <c r="E66" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" t="s">
+        <v>75</v>
+      </c>
+      <c r="G66" t="s">
+        <v>78</v>
+      </c>
+      <c r="H66" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>166</v>
+        <v>8</v>
       </c>
       <c r="B67" t="s">
-        <v>167</v>
+        <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>161</v>
+        <v>10</v>
+      </c>
+      <c r="D67" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" t="s">
+        <v>14</v>
+      </c>
+      <c r="H67" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>109</v>
       </c>
       <c r="B68" t="s">
-        <v>169</v>
+        <v>110</v>
       </c>
       <c r="C68" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
-      <c r="A69" t="s">
-        <v>130</v>
-      </c>
-      <c r="B69" t="s">
-        <v>131</v>
-      </c>
-      <c r="C69" t="s">
-        <v>40</v>
-      </c>
-      <c r="D69" t="s">
-        <v>132</v>
-      </c>
-      <c r="E69" t="s">
-        <v>133</v>
-      </c>
-      <c r="F69" t="s">
-        <v>134</v>
-      </c>
-      <c r="G69" t="s">
-        <v>135</v>
-      </c>
-      <c r="H69" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
-      <c r="A70" t="s">
-        <v>38</v>
-      </c>
-      <c r="B70" t="s">
-        <v>39</v>
-      </c>
-      <c r="C70" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="A71" t="s">
-        <v>76</v>
-      </c>
-      <c r="B71" t="s">
-        <v>77</v>
-      </c>
-      <c r="C71" t="s">
-        <v>78</v>
-      </c>
-      <c r="D71" t="s">
-        <v>79</v>
-      </c>
-      <c r="E71" t="s">
+        <v>111</v>
+      </c>
+      <c r="D68" t="s">
+        <v>112</v>
+      </c>
+      <c r="E68" t="s">
         <v>12</v>
       </c>
-      <c r="F71" t="s">
-        <v>77</v>
-      </c>
-      <c r="G71" t="s">
-        <v>80</v>
-      </c>
-      <c r="H71" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
-      <c r="A72" t="s">
-        <v>8</v>
-      </c>
-      <c r="B72" t="s">
-        <v>9</v>
-      </c>
-      <c r="C72" t="s">
-        <v>10</v>
-      </c>
-      <c r="D72" t="s">
-        <v>11</v>
-      </c>
-      <c r="E72" t="s">
-        <v>12</v>
-      </c>
-      <c r="F72" t="s">
-        <v>13</v>
-      </c>
-      <c r="G72" t="s">
-        <v>14</v>
-      </c>
-      <c r="H72" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
-      <c r="A73" t="s">
-        <v>108</v>
-      </c>
-      <c r="B73" t="s">
-        <v>109</v>
-      </c>
-      <c r="C73" t="s">
-        <v>110</v>
-      </c>
-      <c r="D73" t="s">
-        <v>111</v>
-      </c>
-      <c r="E73" t="s">
-        <v>12</v>
-      </c>
-      <c r="F73" t="s">
-        <v>112</v>
-      </c>
-      <c r="G73" t="s">
+      <c r="F68" t="s">
         <v>113</v>
       </c>
-      <c r="H73" t="s">
+      <c r="G68" t="s">
         <v>114</v>
+      </c>
+      <c r="H68" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix manufacture name in descriptions
R5 and R14 had links instead of names in the manufacture description fields
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="train_horn" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="207">
   <si>
     <t>Reference</t>
   </si>
@@ -475,9 +475,6 @@
     <t>1K</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/supplier-centers/y/yageo</t>
-  </si>
-  <si>
     <t>RC0805FR-071KL</t>
   </si>
   <si>
@@ -632,6 +629,12 @@
   </si>
   <si>
     <t>R25</t>
+  </si>
+  <si>
+    <t>470</t>
+  </si>
+  <si>
+    <t>18650</t>
   </si>
 </sst>
 </file>
@@ -1116,8 +1119,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1476,7 +1480,7 @@
   <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1485,7 +1489,7 @@
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="99.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38" bestFit="1" customWidth="1"/>
@@ -1521,8 +1525,8 @@
       <c r="A2" t="s">
         <v>60</v>
       </c>
-      <c r="B2">
-        <v>18650</v>
+      <c r="B2" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="C2" t="s">
         <v>61</v>
@@ -1571,10 +1575,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C4" t="s">
         <v>41</v>
@@ -1586,21 +1590,21 @@
         <v>43</v>
       </c>
       <c r="F4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4">
+        <v>805</v>
+      </c>
+      <c r="H4" t="s">
         <v>158</v>
-      </c>
-      <c r="G4">
-        <v>805</v>
-      </c>
-      <c r="H4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
         <v>41</v>
@@ -1612,21 +1616,21 @@
         <v>43</v>
       </c>
       <c r="F5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G5">
+        <v>805</v>
+      </c>
+      <c r="H5" t="s">
         <v>158</v>
-      </c>
-      <c r="G5">
-        <v>805</v>
-      </c>
-      <c r="H5" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C6" t="s">
         <v>41</v>
@@ -1638,21 +1642,21 @@
         <v>43</v>
       </c>
       <c r="F6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6">
+        <v>805</v>
+      </c>
+      <c r="H6" t="s">
         <v>158</v>
-      </c>
-      <c r="G6">
-        <v>805</v>
-      </c>
-      <c r="H6" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" t="s">
         <v>41</v>
@@ -1664,21 +1668,21 @@
         <v>43</v>
       </c>
       <c r="F7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7">
+        <v>805</v>
+      </c>
+      <c r="H7" t="s">
         <v>158</v>
-      </c>
-      <c r="G7">
-        <v>805</v>
-      </c>
-      <c r="H7" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C8" t="s">
         <v>41</v>
@@ -1690,21 +1694,21 @@
         <v>43</v>
       </c>
       <c r="F8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G8">
+        <v>805</v>
+      </c>
+      <c r="H8" t="s">
         <v>158</v>
-      </c>
-      <c r="G8">
-        <v>805</v>
-      </c>
-      <c r="H8" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
         <v>41</v>
@@ -1716,21 +1720,21 @@
         <v>43</v>
       </c>
       <c r="F9" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9">
+        <v>805</v>
+      </c>
+      <c r="H9" t="s">
         <v>158</v>
-      </c>
-      <c r="G9">
-        <v>805</v>
-      </c>
-      <c r="H9" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
         <v>41</v>
@@ -1742,13 +1746,13 @@
         <v>43</v>
       </c>
       <c r="F10" t="s">
+        <v>157</v>
+      </c>
+      <c r="G10">
+        <v>805</v>
+      </c>
+      <c r="H10" t="s">
         <v>158</v>
-      </c>
-      <c r="G10">
-        <v>805</v>
-      </c>
-      <c r="H10" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1805,7 +1809,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B13" t="s">
         <v>117</v>
@@ -1831,10 +1835,10 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" t="s">
         <v>156</v>
-      </c>
-      <c r="B14" t="s">
-        <v>157</v>
       </c>
       <c r="C14" t="s">
         <v>41</v>
@@ -1846,18 +1850,18 @@
         <v>43</v>
       </c>
       <c r="F14" t="s">
+        <v>157</v>
+      </c>
+      <c r="G14">
+        <v>805</v>
+      </c>
+      <c r="H14" t="s">
         <v>158</v>
-      </c>
-      <c r="G14">
-        <v>805</v>
-      </c>
-      <c r="H14" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B15" t="s">
         <v>81</v>
@@ -1909,7 +1913,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
@@ -1935,7 +1939,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B18" t="s">
         <v>81</v>
@@ -1961,10 +1965,10 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
         <v>41</v>
@@ -1976,18 +1980,18 @@
         <v>43</v>
       </c>
       <c r="F19" t="s">
+        <v>157</v>
+      </c>
+      <c r="G19">
+        <v>805</v>
+      </c>
+      <c r="H19" t="s">
         <v>158</v>
-      </c>
-      <c r="G19">
-        <v>805</v>
-      </c>
-      <c r="H19" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B20" t="s">
         <v>81</v>
@@ -2013,10 +2017,10 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C21" t="s">
         <v>41</v>
@@ -2028,21 +2032,21 @@
         <v>43</v>
       </c>
       <c r="F21" t="s">
+        <v>157</v>
+      </c>
+      <c r="G21">
+        <v>805</v>
+      </c>
+      <c r="H21" t="s">
         <v>158</v>
-      </c>
-      <c r="G21">
-        <v>805</v>
-      </c>
-      <c r="H21" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C22" t="s">
         <v>41</v>
@@ -2054,13 +2058,13 @@
         <v>43</v>
       </c>
       <c r="F22" t="s">
+        <v>157</v>
+      </c>
+      <c r="G22">
+        <v>805</v>
+      </c>
+      <c r="H22" t="s">
         <v>158</v>
-      </c>
-      <c r="G22">
-        <v>805</v>
-      </c>
-      <c r="H22" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2186,13 +2190,13 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
+        <v>159</v>
+      </c>
+      <c r="B28" t="s">
         <v>160</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>161</v>
-      </c>
-      <c r="C28" t="s">
-        <v>162</v>
       </c>
       <c r="D28" t="s">
         <v>24</v>
@@ -2201,13 +2205,13 @@
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G28">
         <v>1206</v>
       </c>
       <c r="H28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2229,13 +2233,13 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D30" t="s">
         <v>24</v>
@@ -2244,24 +2248,24 @@
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G30">
         <v>1206</v>
       </c>
       <c r="H30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D31" t="s">
         <v>24</v>
@@ -2270,24 +2274,24 @@
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G31">
         <v>1206</v>
       </c>
       <c r="H31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
+        <v>164</v>
+      </c>
+      <c r="B32" t="s">
         <v>165</v>
       </c>
-      <c r="B32" t="s">
-        <v>166</v>
-      </c>
       <c r="C32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D32" t="s">
         <v>24</v>
@@ -2296,24 +2300,24 @@
         <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G32">
         <v>1206</v>
       </c>
       <c r="H32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D33" t="s">
         <v>24</v>
@@ -2322,24 +2326,24 @@
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G33">
         <v>1206</v>
       </c>
       <c r="H33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C34" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D34" t="s">
         <v>24</v>
@@ -2348,24 +2352,24 @@
         <v>25</v>
       </c>
       <c r="F34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G34">
         <v>1206</v>
       </c>
       <c r="H34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D35" t="s">
         <v>24</v>
@@ -2374,13 +2378,13 @@
         <v>25</v>
       </c>
       <c r="F35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G35">
         <v>1206</v>
       </c>
       <c r="H35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2480,7 +2484,7 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B40" t="s">
         <v>33</v>
@@ -2506,7 +2510,7 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B41" t="s">
         <v>22</v>
@@ -2532,7 +2536,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B42" t="s">
         <v>29</v>
@@ -2558,7 +2562,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B43" t="s">
         <v>152</v>
@@ -2570,21 +2574,21 @@
         <v>24</v>
       </c>
       <c r="E43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" t="s">
         <v>153</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43">
+        <v>805</v>
+      </c>
+      <c r="H43" t="s">
         <v>154</v>
-      </c>
-      <c r="G43">
-        <v>805</v>
-      </c>
-      <c r="H43" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B44" t="s">
         <v>33</v>
@@ -2610,7 +2614,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B45" t="s">
         <v>22</v>
@@ -2636,7 +2640,7 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B46" t="s">
         <v>29</v>
@@ -2662,10 +2666,10 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" t="s">
         <v>167</v>
-      </c>
-      <c r="B47" t="s">
-        <v>168</v>
       </c>
       <c r="C47" t="s">
         <v>23</v>
@@ -2677,21 +2681,21 @@
         <v>25</v>
       </c>
       <c r="F47" t="s">
+        <v>168</v>
+      </c>
+      <c r="G47">
+        <v>805</v>
+      </c>
+      <c r="H47" t="s">
         <v>169</v>
-      </c>
-      <c r="G47">
-        <v>805</v>
-      </c>
-      <c r="H47" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B48" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C48" t="s">
         <v>23</v>
@@ -2703,13 +2707,13 @@
         <v>25</v>
       </c>
       <c r="F48" t="s">
+        <v>168</v>
+      </c>
+      <c r="G48">
+        <v>805</v>
+      </c>
+      <c r="H48" t="s">
         <v>169</v>
-      </c>
-      <c r="G48">
-        <v>805</v>
-      </c>
-      <c r="H48" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2740,10 +2744,10 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B50" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C50" t="s">
         <v>23</v>
@@ -2755,21 +2759,21 @@
         <v>25</v>
       </c>
       <c r="F50" t="s">
+        <v>168</v>
+      </c>
+      <c r="G50">
+        <v>805</v>
+      </c>
+      <c r="H50" t="s">
         <v>169</v>
-      </c>
-      <c r="G50">
-        <v>805</v>
-      </c>
-      <c r="H50" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C51" t="s">
         <v>23</v>
@@ -2781,21 +2785,21 @@
         <v>25</v>
       </c>
       <c r="F51" t="s">
+        <v>168</v>
+      </c>
+      <c r="G51">
+        <v>805</v>
+      </c>
+      <c r="H51" t="s">
         <v>169</v>
-      </c>
-      <c r="G51">
-        <v>805</v>
-      </c>
-      <c r="H51" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B52" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C52" t="s">
         <v>23</v>
@@ -2807,21 +2811,21 @@
         <v>25</v>
       </c>
       <c r="F52" t="s">
+        <v>168</v>
+      </c>
+      <c r="G52">
+        <v>805</v>
+      </c>
+      <c r="H52" t="s">
         <v>169</v>
-      </c>
-      <c r="G52">
-        <v>805</v>
-      </c>
-      <c r="H52" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C53" t="s">
         <v>23</v>
@@ -2833,21 +2837,21 @@
         <v>25</v>
       </c>
       <c r="F53" t="s">
+        <v>168</v>
+      </c>
+      <c r="G53">
+        <v>805</v>
+      </c>
+      <c r="H53" t="s">
         <v>169</v>
-      </c>
-      <c r="G53">
-        <v>805</v>
-      </c>
-      <c r="H53" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B54" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C54" t="s">
         <v>23</v>
@@ -2859,21 +2863,21 @@
         <v>25</v>
       </c>
       <c r="F54" t="s">
+        <v>168</v>
+      </c>
+      <c r="G54">
+        <v>805</v>
+      </c>
+      <c r="H54" t="s">
         <v>169</v>
-      </c>
-      <c r="G54">
-        <v>805</v>
-      </c>
-      <c r="H54" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B55" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C55" t="s">
         <v>23</v>
@@ -2885,21 +2889,21 @@
         <v>25</v>
       </c>
       <c r="F55" t="s">
+        <v>168</v>
+      </c>
+      <c r="G55">
+        <v>805</v>
+      </c>
+      <c r="H55" t="s">
         <v>169</v>
-      </c>
-      <c r="G55">
-        <v>805</v>
-      </c>
-      <c r="H55" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>50</v>
       </c>
-      <c r="B56">
-        <v>470</v>
+      <c r="B56" s="1" t="s">
+        <v>205</v>
       </c>
       <c r="C56" t="s">
         <v>23</v>
@@ -2922,7 +2926,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B57" t="s">
         <v>122</v>
@@ -2960,16 +2964,16 @@
         <v>24</v>
       </c>
       <c r="E58" t="s">
+        <v>25</v>
+      </c>
+      <c r="F58" t="s">
         <v>153</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58">
+        <v>805</v>
+      </c>
+      <c r="H58" t="s">
         <v>154</v>
-      </c>
-      <c r="G58">
-        <v>805</v>
-      </c>
-      <c r="H58" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:8">

</xml_diff>